<commit_message>
changes in authirity_modem changes in login changes in department_model changes in login_model changes in config changes in routes changes in home changes in mhome  changes in add_department  changes in add_org changes in footer changes in login  changes in left_menu changes in manage_depart changes in manage_org  changes in signup
</commit_message>
<xml_diff>
--- a/junctionhrms_trackchanges.xlsx
+++ b/junctionhrms_trackchanges.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Design Changes" sheetId="1" r:id="rId1"/>
+    <sheet name="Database changes" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
   <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
     <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
   <si>
     <t>Sno</t>
   </si>
@@ -64,13 +65,55 @@
   </si>
   <si>
     <t>Comment</t>
+  </si>
+  <si>
+    <t>Changes</t>
+  </si>
+  <si>
+    <t>Pages/module</t>
+  </si>
+  <si>
+    <t xml:space="preserve">designation </t>
+  </si>
+  <si>
+    <t>Field Name</t>
+  </si>
+  <si>
+    <t>Designation_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> department_id</t>
+  </si>
+  <si>
+    <t>orgnization</t>
+  </si>
+  <si>
+    <t>Designation_name</t>
+  </si>
+  <si>
+    <t>designation_id</t>
+  </si>
+  <si>
+    <t>designation_name</t>
+  </si>
+  <si>
+    <t>Ankit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">no connectivity b/w department and orgnization after discussion </t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>24/06/15</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -82,6 +125,13 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -113,7 +163,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -122,6 +172,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -394,7 +445,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -404,8 +455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -517,4 +568,104 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:O6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="9.5703125" customWidth="1"/>
+    <col min="2" max="2" width="37" customWidth="1"/>
+    <col min="3" max="3" width="40" customWidth="1"/>
+    <col min="4" max="4" width="37.42578125" customWidth="1"/>
+    <col min="5" max="5" width="27.5703125" customWidth="1"/>
+    <col min="6" max="6" width="36.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+    </row>
+    <row r="2" spans="1:15" ht="30">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
+      <c r="C5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Work on the crm ui module
</commit_message>
<xml_diff>
--- a/junctionhrms_trackchanges.xlsx
+++ b/junctionhrms_trackchanges.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4506"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7755" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Design Changes" sheetId="1" r:id="rId1"/>
     <sheet name="Database changes" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
   <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
     <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="34">
   <si>
     <t>Sno</t>
   </si>
@@ -107,13 +107,50 @@
   </si>
   <si>
     <t>24/06/15</t>
+  </si>
+  <si>
+    <t>.sidebar-menu {</t>
+  </si>
+  <si>
+    <r>
+      <t>width</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF222222"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>: 220px;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>width</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF222222"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>: 340px;</t>
+    </r>
+  </si>
+  <si>
+    <t>sidebar width reduce line 788</t>
+  </si>
+  <si>
+    <t>xenon-core.css</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -135,6 +172,25 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF222222"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FFC80000"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="9"/>
+      <color rgb="FFC80000"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="3">
@@ -163,7 +219,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -173,6 +229,16 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -445,7 +511,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -453,10 +519,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F15"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:O1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -564,6 +631,50 @@
         <v>11</v>
       </c>
     </row>
+    <row r="17" spans="1:7" ht="30">
+      <c r="A17">
+        <v>3</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="B18" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -574,7 +685,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>

</xml_diff>